<commit_message>
Update rebar3 migration documentation.
</commit_message>
<xml_diff>
--- a/docs/Migration to rebar3.xlsx
+++ b/docs/Migration to rebar3.xlsx
@@ -4,22 +4,22 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="45" windowWidth="16275" windowHeight="12090"/>
+    <workbookView xWindow="360" yWindow="45" windowWidth="16275" windowHeight="12090" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="rebar2 -&gt; rebar3" sheetId="1" r:id="rId1"/>
+    <sheet name="Status" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">Sheet1!$A:$B,Sheet1!$1:$1</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">'rebar2 -&gt; rebar3'!$A:$B,'rebar2 -&gt; rebar3'!$1:$1</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="157">
   <si>
     <t>Project</t>
   </si>
@@ -385,12 +385,123 @@
   </si>
   <si>
     <t>compile: src/erlimem_session.erl:none: undefined parse transform 'lager_transform'</t>
+  </si>
+  <si>
+    <t>rebar2</t>
+  </si>
+  <si>
+    <t>rebar3</t>
+  </si>
+  <si>
+    <t>Compile</t>
+  </si>
+  <si>
+    <t>Xref</t>
+  </si>
+  <si>
+    <t>0.3.0</t>
+  </si>
+  <si>
+    <t>2.0.3</t>
+  </si>
+  <si>
+    <t>1.2.0</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>1.7.0</t>
+  </si>
+  <si>
+    <t>&gt; 100</t>
+  </si>
+  <si>
+    <t>1.0.2</t>
+  </si>
+  <si>
+    <t>0.1.0</t>
+  </si>
+  <si>
+    <t>1.68</t>
+  </si>
+  <si>
+    <t>28152…</t>
+  </si>
+  <si>
+    <t>error</t>
+  </si>
+  <si>
+    <t>no longer needed</t>
+  </si>
+  <si>
+    <t>181</t>
+  </si>
+  <si>
+    <t>397</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>now/0</t>
+  </si>
+  <si>
+    <t>shift/reduce</t>
+  </si>
+  <si>
+    <t>i31/1 unused</t>
+  </si>
+  <si>
+    <t>1 ?</t>
+  </si>
+  <si>
+    <t>https://github.com/K2InformaticsGmbH/mimetypes</t>
+  </si>
+  <si>
+    <t>Scripts</t>
+  </si>
+  <si>
+    <t>3/5</t>
+  </si>
+  <si>
+    <t>nok</t>
+  </si>
+  <si>
+    <t>see level 3.1</t>
+  </si>
+  <si>
+    <t>Jenkins</t>
+  </si>
+  <si>
+    <t>Cover final</t>
+  </si>
+  <si>
+    <t>Could Not Find ...\erlscrypt\-f</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>58</t>
+  </si>
+  <si>
+    <t>1.8.0</t>
+  </si>
+  <si>
+    <t>6daca…</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -551,7 +662,7 @@
     <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -595,6 +706,36 @@
     <xf numFmtId="49" fontId="10" fillId="5" borderId="0" xfId="4" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="5" borderId="0" xfId="4" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="4" borderId="0" xfId="3" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="4"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
@@ -911,7 +1052,7 @@
   </sheetPr>
   <dimension ref="A1:P33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -1320,7 +1461,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" ht="14.45" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="18">
         <v>2</v>
       </c>
@@ -1340,7 +1481,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" ht="14.45" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="18">
         <v>2</v>
       </c>
@@ -1377,7 +1518,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" ht="14.45" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="18">
         <v>2</v>
       </c>
@@ -1394,7 +1535,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" ht="14.45" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="17">
         <v>2</v>
       </c>
@@ -1414,7 +1555,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" ht="14.45" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="17">
         <v>3</v>
       </c>
@@ -1443,7 +1584,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" ht="14.45" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="17">
         <v>3</v>
       </c>
@@ -1460,7 +1601,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="24" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" ht="28.9" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="18">
         <v>3</v>
       </c>
@@ -1486,7 +1627,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" ht="14.45" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="17">
         <v>3</v>
       </c>
@@ -1506,7 +1647,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" ht="43.15" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="18">
         <v>3</v>
       </c>
@@ -1553,7 +1694,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" ht="28.9" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="22">
         <v>3</v>
       </c>
@@ -1600,7 +1741,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" ht="14.45" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="17">
         <v>3</v>
       </c>
@@ -1639,7 +1780,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" ht="14.45" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="17">
         <v>4</v>
       </c>
@@ -1659,7 +1800,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" ht="14.45" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="17">
         <v>4</v>
       </c>
@@ -1679,7 +1820,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" ht="14.45" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="17">
         <v>4</v>
       </c>
@@ -1699,7 +1840,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" ht="14.45" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="17">
         <v>4</v>
       </c>
@@ -1729,7 +1870,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="14.45" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="17">
         <v>4</v>
       </c>
@@ -1828,13 +1969,567 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O21" sqref="O21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <cols>
+    <col min="1" max="1" width="5.7109375" style="35" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.7109375" style="27" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.85546875" style="27" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.140625" style="27" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.42578125" style="27" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.5703125" style="27" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4" style="27" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.140625" style="31" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.5703125" style="31" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="34" t="s">
+        <v>118</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>123</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>146</v>
+      </c>
+      <c r="G1" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="26" t="s">
+        <v>124</v>
+      </c>
+      <c r="I1" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" s="30" t="s">
+        <v>150</v>
+      </c>
+      <c r="M1" s="30" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="35">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="E2" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="32" t="s">
+        <v>147</v>
+      </c>
+      <c r="G2" s="32" t="s">
+        <v>135</v>
+      </c>
+      <c r="H2" s="32" t="s">
+        <v>130</v>
+      </c>
+      <c r="I2" s="28" t="s">
+        <v>144</v>
+      </c>
+      <c r="J2" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="31">
+        <v>0.02</v>
+      </c>
+      <c r="L2" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="M2"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="35">
+        <v>2.1</v>
+      </c>
+      <c r="B3" s="33" t="s">
+        <v>80</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D3" s="29" t="s">
+        <v>149</v>
+      </c>
+      <c r="F3"/>
+      <c r="M3"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="35">
+        <v>2.1</v>
+      </c>
+      <c r="B4" s="33" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D4" s="29" t="s">
+        <v>149</v>
+      </c>
+      <c r="F4"/>
+      <c r="M4"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="35">
+        <v>2.1</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5"/>
+      <c r="G5"/>
+      <c r="I5" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="J5"/>
+      <c r="K5" s="18" t="s">
+        <v>153</v>
+      </c>
+      <c r="M5"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="35">
+        <v>2.1</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="E6" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6"/>
+      <c r="G6"/>
+      <c r="I6" s="28" t="s">
+        <v>154</v>
+      </c>
+      <c r="J6" s="28" t="s">
+        <v>153</v>
+      </c>
+      <c r="K6" s="31">
+        <v>0.61</v>
+      </c>
+      <c r="M6"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="35">
+        <v>2.1</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7"/>
+      <c r="G7"/>
+      <c r="H7"/>
+      <c r="I7" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="J7"/>
+      <c r="K7"/>
+      <c r="M7"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="35">
+        <v>2.1</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E8" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8"/>
+      <c r="G8"/>
+      <c r="I8" s="28" t="s">
+        <v>140</v>
+      </c>
+      <c r="J8"/>
+      <c r="K8" s="31">
+        <v>0.4</v>
+      </c>
+      <c r="M8"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="35">
+        <v>2.1</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="E9" s="29" t="s">
+        <v>141</v>
+      </c>
+      <c r="F9" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9"/>
+      <c r="H9"/>
+      <c r="I9" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="J9"/>
+      <c r="K9" s="31">
+        <v>0.43</v>
+      </c>
+      <c r="M9"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="35">
+        <v>2.1</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="F10"/>
+      <c r="M10"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="35">
+        <v>3.1</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="F11"/>
+      <c r="M11"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="35">
+        <v>3.1</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="F12"/>
+      <c r="M12"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="35">
+        <v>3.1</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F13"/>
+      <c r="M13"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="35">
+        <v>3.2</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="E14" s="36" t="s">
+        <v>152</v>
+      </c>
+      <c r="F14"/>
+      <c r="G14"/>
+      <c r="I14" s="28" t="s">
+        <v>139</v>
+      </c>
+      <c r="J14"/>
+      <c r="K14" s="31">
+        <v>0.52</v>
+      </c>
+      <c r="M14"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="35">
+        <v>3.2</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F15"/>
+      <c r="M15"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="35">
+        <v>3.2</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F16"/>
+      <c r="M16"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="35">
+        <v>3.2</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="E17" s="29" t="s">
+        <v>143</v>
+      </c>
+      <c r="F17"/>
+      <c r="M17"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="35">
+        <v>3.2</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F18"/>
+      <c r="M18"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="35">
+        <v>3.2</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="F19"/>
+      <c r="M19"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" s="35">
+        <v>3.2</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E20" s="29" t="s">
+        <v>142</v>
+      </c>
+      <c r="F20"/>
+      <c r="G20"/>
+      <c r="I20" s="28" t="s">
+        <v>138</v>
+      </c>
+      <c r="J20"/>
+      <c r="K20" s="31">
+        <v>0.75</v>
+      </c>
+      <c r="M20"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" s="35">
+        <v>4</v>
+      </c>
+      <c r="B21" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="D21" s="29" t="s">
+        <v>136</v>
+      </c>
+      <c r="F21"/>
+      <c r="M21"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" s="35">
+        <v>4</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="E22" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="F22"/>
+      <c r="G22"/>
+      <c r="I22" s="28" t="s">
+        <v>128</v>
+      </c>
+      <c r="J22"/>
+      <c r="K22" s="31">
+        <v>0.73</v>
+      </c>
+      <c r="M22"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F23"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F24"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F25"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F26"/>
+    </row>
+  </sheetData>
+  <sortState ref="A2:J24">
+    <sortCondition ref="A2:A24"/>
+    <sortCondition ref="B2:B24"/>
+  </sortState>
+  <hyperlinks>
+    <hyperlink ref="B22" r:id="rId1"/>
+    <hyperlink ref="B20" r:id="rId2"/>
+    <hyperlink ref="B19" r:id="rId3"/>
+    <hyperlink ref="B21" r:id="rId4"/>
+    <hyperlink ref="B13" r:id="rId5"/>
+    <hyperlink ref="B17" r:id="rId6"/>
+    <hyperlink ref="B15" r:id="rId7"/>
+    <hyperlink ref="B16" r:id="rId8"/>
+    <hyperlink ref="B14" r:id="rId9"/>
+    <hyperlink ref="B9" r:id="rId10"/>
+    <hyperlink ref="B18" r:id="rId11"/>
+    <hyperlink ref="B3" r:id="rId12"/>
+    <hyperlink ref="B4" r:id="rId13"/>
+    <hyperlink ref="B8" r:id="rId14"/>
+    <hyperlink ref="B5" r:id="rId15"/>
+    <hyperlink ref="B6" r:id="rId16"/>
+    <hyperlink ref="B7" r:id="rId17"/>
+    <hyperlink ref="B2" r:id="rId18"/>
+    <hyperlink ref="B11" r:id="rId19"/>
+    <hyperlink ref="B12" r:id="rId20"/>
+    <hyperlink ref="B10" r:id="rId21"/>
+  </hyperlinks>
+  <printOptions gridLines="1"/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="96" orientation="landscape" r:id="rId22"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;P/&amp;N&amp;R&amp;D</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 

</xml_diff>